<commit_message>
Updated BOM to include a sheet on Electrical, to be populated later
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -8,8 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Mechanical" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Electrical" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
@@ -636,16 +635,4 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
updated BOM with electrical component
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="120" windowWidth="10515" windowHeight="4680" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="180" windowWidth="10515" windowHeight="4620" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Mechanical" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="45">
   <si>
     <t>PUSH BUTTON SWITCH PS-300C1 RED MOMENTARY</t>
   </si>
@@ -105,13 +105,59 @@
   </si>
   <si>
     <t>ALT. SUPPLIER</t>
+  </si>
+  <si>
+    <t>Raspberry Pi Zero</t>
+  </si>
+  <si>
+    <t>CanaKit.com</t>
+  </si>
+  <si>
+    <t>powe bank</t>
+  </si>
+  <si>
+    <t>NCIX.com</t>
+  </si>
+  <si>
+    <t>PIVOS Moju 2600mAh Mobile Charer</t>
+  </si>
+  <si>
+    <t>Adafruit</t>
+  </si>
+  <si>
+    <t>Raspberry Pi Foundation</t>
+  </si>
+  <si>
+    <t>Pivos</t>
+  </si>
+  <si>
+    <t>Nintendo</t>
+  </si>
+  <si>
+    <t>Wiimote</t>
+  </si>
+  <si>
+    <t>Kingston 32Gb sd card</t>
+  </si>
+  <si>
+    <t>SD card with Debian Jesssie lite loaded</t>
+  </si>
+  <si>
+    <t>4mm Screws</t>
+  </si>
+  <si>
+    <t>4mm nuts</t>
+  </si>
+  <si>
+    <t>ribbon cable with 40 pin IDC connector</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
@@ -160,11 +206,12 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -468,10 +515,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -613,6 +660,70 @@
         <v>17</v>
       </c>
       <c r="K4" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6">
+        <v>4</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="K6" s="1" t="s">
         <v>2</v>
       </c>
     </row>
@@ -627,15 +738,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>19</v>
       </c>
@@ -645,15 +756,176 @@
       <c r="C1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="1">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G2" s="4">
+        <v>6.75</v>
+      </c>
+      <c r="H2" t="s">
+        <v>35</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J2" t="s">
+        <v>36</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3">
+        <v>99830</v>
+      </c>
+      <c r="G3" s="4">
+        <v>7.99</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J3" t="s">
+        <v>37</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J4" t="s">
+        <v>38</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G5" s="4">
+        <v>13.99</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F6" t="s">
+        <v>2</v>
+      </c>
+      <c r="G6" t="s">
+        <v>2</v>
+      </c>
+      <c r="H6" t="s">
+        <v>2</v>
+      </c>
+      <c r="I6" t="s">
+        <v>2</v>
+      </c>
+      <c r="J6" t="s">
+        <v>2</v>
+      </c>
+      <c r="K6" t="s">
+        <v>2</v>
+      </c>
+      <c r="L6" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>